<commit_message>
Changed link in BOM
Changed link in BOM to correct capacitor
</commit_message>
<xml_diff>
--- a/Documentation/RC_Car_BOM_v1.0.xlsx
+++ b/Documentation/RC_Car_BOM_v1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-Team/Shared Documents/Server/3 AT Library/WIP/Remote control car adaption/Switch_adapted_remote_controlled_cartoon_car/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-Team/Shared Documents/Server/3 AT Library/Published/Remote control car adaption/Switch_adapted_remote_controlled_cartoon_car/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CE2D98A-5B84-4F0D-8583-CE866E5013F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{5CE2D98A-5B84-4F0D-8583-CE866E5013F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E005B55-6A66-4357-AC40-55446EEE3293}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t>Total Cost</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>https://www.amazon.ca/dp/B00N3HL6F0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/vishay-beyschlag-draloric-bc-components/K103K15X7RH5TL2/286565 </t>
   </si>
 </sst>
 </file>
@@ -831,25 +834,27 @@
   </sheetPr>
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" customWidth="1"/>
-    <col min="7" max="7" width="20.44140625" customWidth="1"/>
-    <col min="8" max="8" width="19.109375" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="89.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="89.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="89.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="36" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:12" ht="35.25" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -863,7 +868,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
@@ -883,12 +888,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -917,7 +922,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -945,7 +950,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -973,7 +978,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -998,7 +1003,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1026,10 +1031,10 @@
         <v>38</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1051,12 +1056,12 @@
         <v>2.7749999999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="26"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
     </row>
-    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>13</v>
       </c>
@@ -1068,7 +1073,7 @@
       <c r="G12" s="22"/>
       <c r="L12" s="8"/>
     </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>14</v>
       </c>
@@ -1091,7 +1096,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1101,21 +1106,21 @@
       </c>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E15" s="17">
         <f t="shared" ref="E15:E16" si="0">(D15/1000)*$B$12</f>
         <v>0</v>
       </c>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E16" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
       <c r="D17" s="19" t="s">
         <v>19</v>
@@ -1126,7 +1131,7 @@
       </c>
       <c r="G17" s="13"/>
     </row>
-    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>20</v>
       </c>
@@ -1142,38 +1147,38 @@
       <c r="K18" s="11"/>
       <c r="L18" s="11"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="28" t="s">
         <v>21</v>
       </c>
@@ -1189,7 +1194,7 @@
       <c r="K26" s="11"/>
       <c r="L26" s="11"/>
     </row>
-    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="29" t="s">
         <v>22</v>
       </c>
@@ -1197,12 +1202,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -1210,7 +1215,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -1218,7 +1223,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -1231,10 +1236,10 @@
     <hyperlink ref="I6" r:id="rId1" xr:uid="{06D5065D-F56C-4459-A5B6-F978671D028C}"/>
     <hyperlink ref="I5" r:id="rId2" xr:uid="{BF0EC09C-9C10-4688-866D-B7E63D9F3BA3}"/>
     <hyperlink ref="I7" r:id="rId3" xr:uid="{1EC2ECC3-A9A1-482F-9227-B7C54DF3D62F}"/>
-    <hyperlink ref="I8" r:id="rId4" xr:uid="{93915BC1-8907-4E55-A5E0-E2C0664AA06A}"/>
-    <hyperlink ref="B29" r:id="rId5" xr:uid="{B95EA35D-EE44-4F80-AB40-BD36660464FB}"/>
-    <hyperlink ref="B31" r:id="rId6" xr:uid="{1B88772E-CD6B-4107-931A-7310840360B6}"/>
-    <hyperlink ref="B32" r:id="rId7" xr:uid="{CF555172-50F8-4971-8A82-744E675A9C36}"/>
+    <hyperlink ref="B29" r:id="rId4" xr:uid="{B95EA35D-EE44-4F80-AB40-BD36660464FB}"/>
+    <hyperlink ref="B31" r:id="rId5" xr:uid="{1B88772E-CD6B-4107-931A-7310840360B6}"/>
+    <hyperlink ref="B32" r:id="rId6" xr:uid="{CF555172-50F8-4971-8A82-744E675A9C36}"/>
+    <hyperlink ref="I8" r:id="rId7" xr:uid="{E7E5A80F-FC1C-4684-A155-C68A636333F8}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -1243,6 +1248,43 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="38b325e6-602c-452a-8617-173bf47082c5" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cf100d1-0775-4feb-8634-62999c4541bc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="38b325e6-602c-452a-8617-173bf47082c5">
+      <UserInfo>
+        <DisplayName>Courtney Cameron</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Josie Versloot</DisplayName>
+        <AccountId>503</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Shanelle Waiting</DisplayName>
+        <AccountId>21</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100456CAEA290209545A9F8681F83603874" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d27786a72e09a52c769a64d5f7eeaa24">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8cf100d1-0775-4feb-8634-62999c4541bc" xmlns:ns3="38b325e6-602c-452a-8617-173bf47082c5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="03ae89856d271009074f70b56337b48d" ns2:_="" ns3:_="">
     <xsd:import namespace="8cf100d1-0775-4feb-8634-62999c4541bc"/>
@@ -1479,44 +1521,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="38b325e6-602c-452a-8617-173bf47082c5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="8cf100d1-0775-4feb-8634-62999c4541bc"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="38b325e6-602c-452a-8617-173bf47082c5" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cf100d1-0775-4feb-8634-62999c4541bc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="38b325e6-602c-452a-8617-173bf47082c5">
-      <UserInfo>
-        <DisplayName>Courtney Cameron</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Josie Versloot</DisplayName>
-        <AccountId>503</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Shanelle Waiting</DisplayName>
-        <AccountId>21</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99BECD52-63A8-454F-82E6-6195B786F95C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1533,29 +1563,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="38b325e6-602c-452a-8617-173bf47082c5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="8cf100d1-0775-4feb-8634-62999c4541bc"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>